<commit_message>
refactor: add case-insensitivity to faculty name; add control tasks achievement check; add new tests
</commit_message>
<xml_diff>
--- a/OnlineCoursesAnalyzerTests/Data/DataHandlerTestsData/EducationalAchievmentDataWithManyNotMathmechStudentsErrorRows.xlsx
+++ b/OnlineCoursesAnalyzerTests/Data/DataHandlerTestsData/EducationalAchievmentDataWithManyNotMathmechStudentsErrorRows.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="263">
   <si>
     <t>Student ID</t>
   </si>
@@ -204,9 +204,6 @@
     <t>0.9</t>
   </si>
   <si>
-    <t>0.887012987013</t>
-  </si>
-  <si>
     <t>st000004@student.spbu.ru</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>0.94696969697</t>
-  </si>
-  <si>
     <t>st000005</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t>0.875</t>
   </si>
   <si>
-    <t>0.873484848485</t>
-  </si>
-  <si>
     <t>verified_18.12.21_медики</t>
   </si>
   <si>
@@ -258,9 +249,6 @@
     <t>st000008</t>
   </si>
   <si>
-    <t>0.892424242424</t>
-  </si>
-  <si>
     <t>st000009@student.spbu.ru</t>
   </si>
   <si>
@@ -270,9 +258,6 @@
     <t>0.88</t>
   </si>
   <si>
-    <t>0.879545454545</t>
-  </si>
-  <si>
     <t>st000010@student.spbu.ru</t>
   </si>
   <si>
@@ -282,9 +267,6 @@
     <t>0.99</t>
   </si>
   <si>
-    <t>0.990909090909</t>
-  </si>
-  <si>
     <t>verified_07.12.21_матмех</t>
   </si>
   <si>
@@ -306,18 +288,12 @@
     <t>st000013</t>
   </si>
   <si>
-    <t>0.988636363636</t>
-  </si>
-  <si>
     <t>st000014@student.spbu.ru</t>
   </si>
   <si>
     <t>st000014</t>
   </si>
   <si>
-    <t>0.901515151515</t>
-  </si>
-  <si>
     <t>st000015@student.spbu.ru</t>
   </si>
   <si>
@@ -357,9 +333,6 @@
     <t>0.91</t>
   </si>
   <si>
-    <t>0.909090909091</t>
-  </si>
-  <si>
     <t>st000021@student.spbu.ru</t>
   </si>
   <si>
@@ -378,9 +351,6 @@
     <t>0.375</t>
   </si>
   <si>
-    <t>0.402164502165</t>
-  </si>
-  <si>
     <t>st000022@student.spbu.ru</t>
   </si>
   <si>
@@ -393,9 +363,6 @@
     <t>st000023</t>
   </si>
   <si>
-    <t>0.992424242424</t>
-  </si>
-  <si>
     <t>st000024@student.spbu.ru</t>
   </si>
   <si>
@@ -420,9 +387,6 @@
     <t>0.8</t>
   </si>
   <si>
-    <t>0.970454545455</t>
-  </si>
-  <si>
     <t>st000027@student.spbu.ru</t>
   </si>
   <si>
@@ -447,9 +411,6 @@
     <t>0.75</t>
   </si>
   <si>
-    <t>0.936363636364</t>
-  </si>
-  <si>
     <t>st000030@student.spbu.ru</t>
   </si>
   <si>
@@ -504,9 +465,6 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>0.819696969697</t>
-  </si>
-  <si>
     <t>st000038@student.spbu.ru</t>
   </si>
   <si>
@@ -528,18 +486,12 @@
     <t>0.6</t>
   </si>
   <si>
-    <t>0.931818181818</t>
-  </si>
-  <si>
     <t>st000041@student.spbu.ru</t>
   </si>
   <si>
     <t>st000041</t>
   </si>
   <si>
-    <t>0.89696969697</t>
-  </si>
-  <si>
     <t>verified_07.12.21_физика</t>
   </si>
   <si>
@@ -847,6 +799,15 @@
   </si>
   <si>
     <t>st000099</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.60</t>
   </si>
 </sst>
 </file>
@@ -882,8 +843,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1166,13 +1130,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U48" sqref="U44:U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1339,7 +1305,7 @@
         <v>38</v>
       </c>
       <c r="U2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V2" t="s">
         <v>38</v>
@@ -1353,8 +1319,8 @@
       <c r="Y2" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" t="s">
-        <v>38</v>
+      <c r="Z2" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA2" t="s">
         <v>40</v>
@@ -1437,7 +1403,7 @@
         <v>38</v>
       </c>
       <c r="U3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V3" t="s">
         <v>38</v>
@@ -1451,8 +1417,8 @@
       <c r="Y3" t="s">
         <v>38</v>
       </c>
-      <c r="Z3" t="s">
-        <v>38</v>
+      <c r="Z3" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA3" t="s">
         <v>40</v>
@@ -1549,8 +1515,8 @@
       <c r="Y4" t="s">
         <v>38</v>
       </c>
-      <c r="Z4" t="s">
-        <v>38</v>
+      <c r="Z4" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA4" t="s">
         <v>52</v>
@@ -1633,7 +1599,7 @@
         <v>50</v>
       </c>
       <c r="U5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="V5" t="s">
         <v>51</v>
@@ -1647,8 +1613,8 @@
       <c r="Y5" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" t="s">
-        <v>38</v>
+      <c r="Z5" s="1">
+        <v>1</v>
       </c>
       <c r="AA5" t="s">
         <v>52</v>
@@ -1677,10 +1643,10 @@
         <v>2714100</v>
       </c>
       <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
@@ -1692,7 +1658,7 @@
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6">
         <v>61</v>
@@ -1713,20 +1679,20 @@
         <v>50</v>
       </c>
       <c r="N6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R6" t="s">
         <v>65</v>
       </c>
-      <c r="O6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R6" t="s">
-        <v>66</v>
-      </c>
       <c r="S6" t="s">
         <v>50</v>
       </c>
@@ -1734,7 +1700,7 @@
         <v>50</v>
       </c>
       <c r="U6" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="V6" t="s">
         <v>51</v>
@@ -1748,8 +1714,8 @@
       <c r="Y6" t="s">
         <v>38</v>
       </c>
-      <c r="Z6" t="s">
-        <v>38</v>
+      <c r="Z6" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA6" t="s">
         <v>52</v>
@@ -1778,7 +1744,7 @@
         <v>2692257</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>35</v>
@@ -1790,7 +1756,7 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7">
         <v>30</v>
@@ -1811,13 +1777,13 @@
         <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O7" t="s">
         <v>50</v>
       </c>
       <c r="P7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q7" t="s">
         <v>50</v>
@@ -1832,7 +1798,7 @@
         <v>50</v>
       </c>
       <c r="U7" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="V7" t="s">
         <v>51</v>
@@ -1846,11 +1812,11 @@
       <c r="Y7" t="s">
         <v>51</v>
       </c>
-      <c r="Z7" t="s">
-        <v>38</v>
+      <c r="Z7" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB7" t="s">
         <v>53</v>
@@ -1876,7 +1842,7 @@
         <v>2692263</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -1944,8 +1910,8 @@
       <c r="Y8" t="s">
         <v>38</v>
       </c>
-      <c r="Z8" t="s">
-        <v>38</v>
+      <c r="Z8" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA8" t="s">
         <v>52</v>
@@ -1974,10 +1940,10 @@
         <v>2692268</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -2028,7 +1994,7 @@
         <v>50</v>
       </c>
       <c r="U9" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="V9" t="s">
         <v>51</v>
@@ -2042,9 +2008,7 @@
       <c r="Y9" t="s">
         <v>38</v>
       </c>
-      <c r="Z9" t="s">
-        <v>38</v>
-      </c>
+      <c r="Z9" s="1"/>
       <c r="AA9" t="s">
         <v>52</v>
       </c>
@@ -2072,10 +2036,10 @@
         <v>2692272</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>35</v>
@@ -2108,7 +2072,7 @@
         <v>50</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O10" t="s">
         <v>50</v>
@@ -2129,7 +2093,7 @@
         <v>50</v>
       </c>
       <c r="U10" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="V10" t="s">
         <v>51</v>
@@ -2143,11 +2107,11 @@
       <c r="Y10" t="s">
         <v>51</v>
       </c>
-      <c r="Z10" t="s">
-        <v>38</v>
+      <c r="Z10" s="1">
+        <v>1</v>
       </c>
       <c r="AA10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="AB10" t="s">
         <v>53</v>
@@ -2173,10 +2137,10 @@
         <v>2692300</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -2188,7 +2152,7 @@
         <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H11">
         <v>100</v>
@@ -2212,7 +2176,7 @@
         <v>50</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P11" t="s">
         <v>50</v>
@@ -2230,7 +2194,7 @@
         <v>50</v>
       </c>
       <c r="U11" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="V11" t="s">
         <v>51</v>
@@ -2244,8 +2208,8 @@
       <c r="Y11" t="s">
         <v>38</v>
       </c>
-      <c r="Z11" t="s">
-        <v>38</v>
+      <c r="Z11" s="1">
+        <v>1</v>
       </c>
       <c r="AA11" t="s">
         <v>52</v>
@@ -2274,10 +2238,10 @@
         <v>2686863</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
@@ -2289,7 +2253,7 @@
         <v>37</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
         <v>39</v>
@@ -2331,7 +2295,7 @@
         <v>50</v>
       </c>
       <c r="U12" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="V12" t="s">
         <v>51</v>
@@ -2345,11 +2309,11 @@
       <c r="Y12" t="s">
         <v>51</v>
       </c>
-      <c r="Z12" t="s">
-        <v>38</v>
+      <c r="Z12" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA12" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB12" t="s">
         <v>53</v>
@@ -2375,10 +2339,10 @@
         <v>2692319</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -2411,7 +2375,7 @@
         <v>50</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O13" t="s">
         <v>50</v>
@@ -2432,7 +2396,7 @@
         <v>50</v>
       </c>
       <c r="U13" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="V13" t="s">
         <v>51</v>
@@ -2446,11 +2410,11 @@
       <c r="Y13" t="s">
         <v>51</v>
       </c>
-      <c r="Z13" t="s">
-        <v>38</v>
+      <c r="Z13" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB13" t="s">
         <v>53</v>
@@ -2476,10 +2440,10 @@
         <v>2686868</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -2533,7 +2497,7 @@
         <v>38</v>
       </c>
       <c r="U14" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V14" t="s">
         <v>51</v>
@@ -2547,11 +2511,11 @@
       <c r="Y14" t="s">
         <v>51</v>
       </c>
-      <c r="Z14" t="s">
-        <v>38</v>
+      <c r="Z14" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB14" t="s">
         <v>48</v>
@@ -2577,10 +2541,10 @@
         <v>2692326</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -2592,7 +2556,7 @@
         <v>37</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H15">
         <v>100</v>
@@ -2619,7 +2583,7 @@
         <v>50</v>
       </c>
       <c r="P15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q15" t="s">
         <v>50</v>
@@ -2634,7 +2598,7 @@
         <v>50</v>
       </c>
       <c r="U15" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="V15" t="s">
         <v>51</v>
@@ -2648,11 +2612,11 @@
       <c r="Y15" t="s">
         <v>51</v>
       </c>
-      <c r="Z15" t="s">
-        <v>38</v>
+      <c r="Z15" s="1">
+        <v>1</v>
       </c>
       <c r="AA15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB15" t="s">
         <v>53</v>
@@ -2678,10 +2642,10 @@
         <v>2692329</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>35</v>
@@ -2714,7 +2678,7 @@
         <v>50</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O16" t="s">
         <v>50</v>
@@ -2735,7 +2699,7 @@
         <v>50</v>
       </c>
       <c r="U16" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V16" t="s">
         <v>51</v>
@@ -2749,11 +2713,11 @@
       <c r="Y16" t="s">
         <v>51</v>
       </c>
-      <c r="Z16" t="s">
-        <v>38</v>
+      <c r="Z16" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA16" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB16" t="s">
         <v>53</v>
@@ -2779,10 +2743,10 @@
         <v>2692333</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -2836,7 +2800,7 @@
         <v>38</v>
       </c>
       <c r="U17" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V17" t="s">
         <v>51</v>
@@ -2850,11 +2814,11 @@
       <c r="Y17" t="s">
         <v>51</v>
       </c>
-      <c r="Z17" t="s">
-        <v>38</v>
+      <c r="Z17" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB17" t="s">
         <v>48</v>
@@ -2880,10 +2844,10 @@
         <v>2686875</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
@@ -2937,7 +2901,7 @@
         <v>38</v>
       </c>
       <c r="U18" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V18" t="s">
         <v>51</v>
@@ -2951,11 +2915,11 @@
       <c r="Y18" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" t="s">
-        <v>38</v>
+      <c r="Z18" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB18" t="s">
         <v>48</v>
@@ -2981,10 +2945,10 @@
         <v>2692341</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -3017,7 +2981,7 @@
         <v>50</v>
       </c>
       <c r="N19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O19" t="s">
         <v>50</v>
@@ -3038,7 +3002,7 @@
         <v>50</v>
       </c>
       <c r="U19" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V19" t="s">
         <v>51</v>
@@ -3052,11 +3016,11 @@
       <c r="Y19" t="s">
         <v>38</v>
       </c>
-      <c r="Z19" t="s">
-        <v>38</v>
+      <c r="Z19" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB19" t="s">
         <v>53</v>
@@ -3082,10 +3046,10 @@
         <v>2686883</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
         <v>35</v>
@@ -3118,7 +3082,7 @@
         <v>50</v>
       </c>
       <c r="N20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O20" t="s">
         <v>50</v>
@@ -3139,7 +3103,7 @@
         <v>50</v>
       </c>
       <c r="U20" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V20" t="s">
         <v>51</v>
@@ -3153,11 +3117,11 @@
       <c r="Y20" t="s">
         <v>51</v>
       </c>
-      <c r="Z20" t="s">
-        <v>38</v>
+      <c r="Z20" s="1">
+        <v>1</v>
       </c>
       <c r="AA20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB20" t="s">
         <v>53</v>
@@ -3183,10 +3147,10 @@
         <v>2686888</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
@@ -3219,7 +3183,7 @@
         <v>50</v>
       </c>
       <c r="N21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O21" t="s">
         <v>50</v>
@@ -3240,7 +3204,7 @@
         <v>50</v>
       </c>
       <c r="U21" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V21" t="s">
         <v>51</v>
@@ -3254,11 +3218,11 @@
       <c r="Y21" t="s">
         <v>51</v>
       </c>
-      <c r="Z21" t="s">
-        <v>38</v>
+      <c r="Z21" s="1">
+        <v>1</v>
       </c>
       <c r="AA21" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB21" t="s">
         <v>53</v>
@@ -3284,10 +3248,10 @@
         <v>2692388</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
         <v>35</v>
@@ -3299,7 +3263,7 @@
         <v>37</v>
       </c>
       <c r="G22" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H22" t="s">
         <v>39</v>
@@ -3341,7 +3305,7 @@
         <v>50</v>
       </c>
       <c r="U22" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="V22" t="s">
         <v>51</v>
@@ -3355,11 +3319,11 @@
       <c r="Y22" t="s">
         <v>38</v>
       </c>
-      <c r="Z22" t="s">
-        <v>38</v>
+      <c r="Z22" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB22" t="s">
         <v>53</v>
@@ -3385,10 +3349,10 @@
         <v>2692390</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
@@ -3400,7 +3364,7 @@
         <v>37</v>
       </c>
       <c r="G23" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H23" t="s">
         <v>47</v>
@@ -3421,13 +3385,13 @@
         <v>59</v>
       </c>
       <c r="N23" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="O23" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="P23" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="Q23" t="s">
         <v>38</v>
@@ -3442,7 +3406,7 @@
         <v>38</v>
       </c>
       <c r="U23" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
       <c r="V23" t="s">
         <v>51</v>
@@ -3456,11 +3420,11 @@
       <c r="Y23" t="s">
         <v>51</v>
       </c>
-      <c r="Z23" t="s">
-        <v>38</v>
+      <c r="Z23" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA23" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB23" t="s">
         <v>53</v>
@@ -3486,10 +3450,10 @@
         <v>2692403</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
         <v>35</v>
@@ -3522,7 +3486,7 @@
         <v>50</v>
       </c>
       <c r="N24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O24" t="s">
         <v>50</v>
@@ -3543,7 +3507,7 @@
         <v>50</v>
       </c>
       <c r="U24" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="V24" t="s">
         <v>51</v>
@@ -3557,11 +3521,11 @@
       <c r="Y24" t="s">
         <v>51</v>
       </c>
-      <c r="Z24" t="s">
-        <v>38</v>
+      <c r="Z24" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB24" t="s">
         <v>53</v>
@@ -3587,10 +3551,10 @@
         <v>2686913</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
         <v>35</v>
@@ -3602,7 +3566,7 @@
         <v>37</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H25">
         <v>100</v>
@@ -3623,7 +3587,7 @@
         <v>50</v>
       </c>
       <c r="N25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O25" t="s">
         <v>50</v>
@@ -3644,7 +3608,7 @@
         <v>50</v>
       </c>
       <c r="U25" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="V25" t="s">
         <v>51</v>
@@ -3658,11 +3622,11 @@
       <c r="Y25" t="s">
         <v>51</v>
       </c>
-      <c r="Z25" t="s">
-        <v>38</v>
+      <c r="Z25" s="1">
+        <v>1</v>
       </c>
       <c r="AA25" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB25" t="s">
         <v>53</v>
@@ -3688,10 +3652,10 @@
         <v>2692423</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
@@ -3703,7 +3667,7 @@
         <v>37</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H26">
         <v>61</v>
@@ -3745,7 +3709,7 @@
         <v>50</v>
       </c>
       <c r="U26" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="V26" t="s">
         <v>51</v>
@@ -3759,11 +3723,11 @@
       <c r="Y26" t="s">
         <v>38</v>
       </c>
-      <c r="Z26" t="s">
-        <v>38</v>
+      <c r="Z26" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA26" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB26" t="s">
         <v>53</v>
@@ -3789,10 +3753,10 @@
         <v>2686918</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D27" t="s">
         <v>35</v>
@@ -3804,7 +3768,7 @@
         <v>37</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H27">
         <v>30</v>
@@ -3825,7 +3789,7 @@
         <v>50</v>
       </c>
       <c r="N27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O27" t="s">
         <v>50</v>
@@ -3846,7 +3810,7 @@
         <v>50</v>
       </c>
       <c r="U27" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="V27" t="s">
         <v>51</v>
@@ -3860,11 +3824,11 @@
       <c r="Y27" t="s">
         <v>51</v>
       </c>
-      <c r="Z27" t="s">
-        <v>38</v>
+      <c r="Z27" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB27" t="s">
         <v>53</v>
@@ -3890,10 +3854,10 @@
         <v>2714149</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
@@ -3905,7 +3869,7 @@
         <v>37</v>
       </c>
       <c r="G28" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="H28">
         <v>40</v>
@@ -3929,7 +3893,7 @@
         <v>50</v>
       </c>
       <c r="O28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P28" t="s">
         <v>50</v>
@@ -3938,7 +3902,7 @@
         <v>50</v>
       </c>
       <c r="R28" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="S28" t="s">
         <v>50</v>
@@ -3947,7 +3911,7 @@
         <v>50</v>
       </c>
       <c r="U28" t="s">
-        <v>133</v>
+        <v>50</v>
       </c>
       <c r="V28" t="s">
         <v>51</v>
@@ -3961,11 +3925,11 @@
       <c r="Y28" t="s">
         <v>51</v>
       </c>
-      <c r="Z28" t="s">
-        <v>38</v>
+      <c r="Z28" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA28" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB28" t="s">
         <v>53</v>
@@ -3991,10 +3955,10 @@
         <v>2684311</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
@@ -4048,7 +4012,7 @@
         <v>38</v>
       </c>
       <c r="U29" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V29" t="s">
         <v>51</v>
@@ -4062,11 +4026,11 @@
       <c r="Y29" t="s">
         <v>51</v>
       </c>
-      <c r="Z29" t="s">
-        <v>38</v>
+      <c r="Z29" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB29" t="s">
         <v>48</v>
@@ -4092,10 +4056,10 @@
         <v>2692485</v>
       </c>
       <c r="B30" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
         <v>35</v>
@@ -4107,7 +4071,7 @@
         <v>37</v>
       </c>
       <c r="G30" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H30">
         <v>100</v>
@@ -4149,7 +4113,7 @@
         <v>50</v>
       </c>
       <c r="U30" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="V30" t="s">
         <v>51</v>
@@ -4163,11 +4127,11 @@
       <c r="Y30" t="s">
         <v>38</v>
       </c>
-      <c r="Z30" t="s">
-        <v>38</v>
+      <c r="Z30" s="1">
+        <v>1</v>
       </c>
       <c r="AA30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB30" t="s">
         <v>53</v>
@@ -4193,10 +4157,10 @@
         <v>2692486</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
         <v>35</v>
@@ -4208,7 +4172,7 @@
         <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="H31">
         <v>100</v>
@@ -4220,7 +4184,7 @@
         <v>50</v>
       </c>
       <c r="K31" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="L31" t="s">
         <v>50</v>
@@ -4232,10 +4196,10 @@
         <v>50</v>
       </c>
       <c r="O31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q31" t="s">
         <v>60</v>
@@ -4250,7 +4214,7 @@
         <v>50</v>
       </c>
       <c r="U31" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
       <c r="V31" t="s">
         <v>51</v>
@@ -4264,11 +4228,11 @@
       <c r="Y31" t="s">
         <v>51</v>
       </c>
-      <c r="Z31" t="s">
-        <v>38</v>
+      <c r="Z31" s="1">
+        <v>1</v>
       </c>
       <c r="AA31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB31" t="s">
         <v>53</v>
@@ -4294,10 +4258,10 @@
         <v>2692491</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D32" t="s">
         <v>35</v>
@@ -4365,11 +4329,11 @@
       <c r="Y32" t="s">
         <v>38</v>
       </c>
-      <c r="Z32" t="s">
-        <v>38</v>
+      <c r="Z32" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB32" t="s">
         <v>53</v>
@@ -4395,10 +4359,10 @@
         <v>2692502</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
@@ -4431,7 +4395,7 @@
         <v>50</v>
       </c>
       <c r="N33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O33" t="s">
         <v>50</v>
@@ -4452,7 +4416,7 @@
         <v>50</v>
       </c>
       <c r="U33" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V33" t="s">
         <v>51</v>
@@ -4466,11 +4430,11 @@
       <c r="Y33" t="s">
         <v>38</v>
       </c>
-      <c r="Z33" t="s">
-        <v>38</v>
+      <c r="Z33" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA33" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB33" t="s">
         <v>53</v>
@@ -4496,10 +4460,10 @@
         <v>2692549</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D34" t="s">
         <v>35</v>
@@ -4511,7 +4475,7 @@
         <v>37</v>
       </c>
       <c r="G34" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H34">
         <v>90</v>
@@ -4553,7 +4517,7 @@
         <v>50</v>
       </c>
       <c r="U34" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="V34" t="s">
         <v>51</v>
@@ -4567,11 +4531,11 @@
       <c r="Y34" t="s">
         <v>38</v>
       </c>
-      <c r="Z34" t="s">
-        <v>38</v>
+      <c r="Z34" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA34" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB34" t="s">
         <v>53</v>
@@ -4597,10 +4561,10 @@
         <v>2686949</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
         <v>35</v>
@@ -4633,7 +4597,7 @@
         <v>50</v>
       </c>
       <c r="N35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O35" t="s">
         <v>50</v>
@@ -4654,7 +4618,7 @@
         <v>50</v>
       </c>
       <c r="U35" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="V35" t="s">
         <v>51</v>
@@ -4668,11 +4632,11 @@
       <c r="Y35" t="s">
         <v>51</v>
       </c>
-      <c r="Z35" t="s">
-        <v>38</v>
+      <c r="Z35" s="1">
+        <v>1</v>
       </c>
       <c r="AA35" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB35" t="s">
         <v>53</v>
@@ -4698,10 +4662,10 @@
         <v>2692560</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
         <v>35</v>
@@ -4769,11 +4733,11 @@
       <c r="Y36" t="s">
         <v>51</v>
       </c>
-      <c r="Z36" t="s">
-        <v>38</v>
+      <c r="Z36" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA36" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB36" t="s">
         <v>53</v>
@@ -4799,10 +4763,10 @@
         <v>2692563</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
         <v>35</v>
@@ -4814,7 +4778,7 @@
         <v>37</v>
       </c>
       <c r="G37" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H37">
         <v>30</v>
@@ -4856,7 +4820,7 @@
         <v>50</v>
       </c>
       <c r="U37" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="V37" t="s">
         <v>51</v>
@@ -4870,11 +4834,11 @@
       <c r="Y37" t="s">
         <v>38</v>
       </c>
-      <c r="Z37" t="s">
-        <v>38</v>
+      <c r="Z37" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB37" t="s">
         <v>53</v>
@@ -4900,10 +4864,10 @@
         <v>2692580</v>
       </c>
       <c r="B38" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
@@ -4915,7 +4879,7 @@
         <v>37</v>
       </c>
       <c r="G38" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H38">
         <v>40</v>
@@ -4942,7 +4906,7 @@
         <v>50</v>
       </c>
       <c r="P38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q38" t="s">
         <v>50</v>
@@ -4957,7 +4921,7 @@
         <v>50</v>
       </c>
       <c r="U38" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="V38" t="s">
         <v>51</v>
@@ -4971,11 +4935,11 @@
       <c r="Y38" t="s">
         <v>51</v>
       </c>
-      <c r="Z38" t="s">
-        <v>38</v>
+      <c r="Z38" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA38" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB38" t="s">
         <v>53</v>
@@ -5001,10 +4965,10 @@
         <v>2692585</v>
       </c>
       <c r="B39" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D39" t="s">
         <v>35</v>
@@ -5016,7 +4980,7 @@
         <v>37</v>
       </c>
       <c r="G39" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H39">
         <v>80</v>
@@ -5031,13 +4995,13 @@
         <v>38</v>
       </c>
       <c r="L39" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="M39" t="s">
         <v>50</v>
       </c>
       <c r="N39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O39" t="s">
         <v>50</v>
@@ -5058,7 +5022,7 @@
         <v>50</v>
       </c>
       <c r="U39" t="s">
-        <v>161</v>
+        <v>50</v>
       </c>
       <c r="V39" t="s">
         <v>51</v>
@@ -5072,11 +5036,11 @@
       <c r="Y39" t="s">
         <v>38</v>
       </c>
-      <c r="Z39" t="s">
-        <v>38</v>
+      <c r="Z39" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA39" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB39" t="s">
         <v>53</v>
@@ -5102,10 +5066,10 @@
         <v>2686959</v>
       </c>
       <c r="B40" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
         <v>35</v>
@@ -5159,7 +5123,7 @@
         <v>38</v>
       </c>
       <c r="U40" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="V40" t="s">
         <v>51</v>
@@ -5173,11 +5137,11 @@
       <c r="Y40" t="s">
         <v>51</v>
       </c>
-      <c r="Z40" t="s">
-        <v>38</v>
+      <c r="Z40" s="1">
+        <v>1</v>
       </c>
       <c r="AA40" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB40" t="s">
         <v>48</v>
@@ -5203,10 +5167,10 @@
         <v>2692588</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D41" t="s">
         <v>35</v>
@@ -5239,7 +5203,7 @@
         <v>50</v>
       </c>
       <c r="N41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O41" t="s">
         <v>50</v>
@@ -5260,7 +5224,7 @@
         <v>50</v>
       </c>
       <c r="U41" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="V41" t="s">
         <v>51</v>
@@ -5274,11 +5238,11 @@
       <c r="Y41" t="s">
         <v>51</v>
       </c>
-      <c r="Z41" t="s">
-        <v>38</v>
+      <c r="Z41" s="1">
+        <v>1</v>
       </c>
       <c r="AA41" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB41" t="s">
         <v>53</v>
@@ -5304,10 +5268,10 @@
         <v>2692592</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -5319,7 +5283,7 @@
         <v>37</v>
       </c>
       <c r="G42" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H42" t="s">
         <v>47</v>
@@ -5331,10 +5295,10 @@
         <v>50</v>
       </c>
       <c r="K42" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="L42" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="M42" t="s">
         <v>50</v>
@@ -5361,7 +5325,7 @@
         <v>50</v>
       </c>
       <c r="U42" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="V42" t="s">
         <v>51</v>
@@ -5375,11 +5339,11 @@
       <c r="Y42" t="s">
         <v>38</v>
       </c>
-      <c r="Z42" t="s">
-        <v>38</v>
+      <c r="Z42" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA42" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AB42" t="s">
         <v>53</v>
@@ -5405,10 +5369,10 @@
         <v>2686969</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C43" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D43" t="s">
         <v>35</v>
@@ -5420,7 +5384,7 @@
         <v>37</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H43">
         <v>90</v>
@@ -5432,22 +5396,22 @@
         <v>50</v>
       </c>
       <c r="K43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L43" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="M43" t="s">
         <v>50</v>
       </c>
       <c r="N43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q43" t="s">
         <v>50</v>
@@ -5462,7 +5426,7 @@
         <v>50</v>
       </c>
       <c r="U43" t="s">
-        <v>172</v>
+        <v>50</v>
       </c>
       <c r="V43" t="s">
         <v>51</v>
@@ -5476,11 +5440,11 @@
       <c r="Y43" t="s">
         <v>51</v>
       </c>
-      <c r="Z43" t="s">
-        <v>38</v>
+      <c r="Z43" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA43" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="AB43" t="s">
         <v>53</v>
@@ -5502,26 +5466,31 @@
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Z44" s="1"/>
       <c r="AA44" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Z45" s="1"/>
       <c r="AA45" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Z46" s="1"/>
       <c r="AA46" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Z47" s="1"/>
       <c r="AA47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="Z48" s="1"/>
       <c r="AA48" t="s">
         <v>52</v>
       </c>
@@ -5531,10 +5500,10 @@
         <v>2949640.713</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="D49" t="s">
         <v>35</v>
@@ -5546,7 +5515,7 @@
         <v>37</v>
       </c>
       <c r="G49" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H49">
         <v>100</v>
@@ -5602,8 +5571,8 @@
       <c r="Y49" t="s">
         <v>38</v>
       </c>
-      <c r="Z49" t="s">
-        <v>38</v>
+      <c r="Z49" s="1">
+        <v>1</v>
       </c>
       <c r="AA49" t="s">
         <v>52</v>
@@ -5632,10 +5601,10 @@
         <v>2964123.193</v>
       </c>
       <c r="B50" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D50" t="s">
         <v>35</v>
@@ -5703,8 +5672,8 @@
       <c r="Y50" t="s">
         <v>38</v>
       </c>
-      <c r="Z50" t="s">
-        <v>38</v>
+      <c r="Z50" s="1">
+        <v>1</v>
       </c>
       <c r="AA50" t="s">
         <v>52</v>
@@ -5733,10 +5702,10 @@
         <v>2978605.673</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D51" t="s">
         <v>35</v>
@@ -5804,8 +5773,8 @@
       <c r="Y51" t="s">
         <v>38</v>
       </c>
-      <c r="Z51" t="s">
-        <v>38</v>
+      <c r="Z51" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA51" t="s">
         <v>52</v>
@@ -5834,10 +5803,10 @@
         <v>2993088.1529999999</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D52" t="s">
         <v>35</v>
@@ -5849,7 +5818,7 @@
         <v>37</v>
       </c>
       <c r="G52" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H52" t="s">
         <v>47</v>
@@ -5905,8 +5874,8 @@
       <c r="Y52" t="s">
         <v>38</v>
       </c>
-      <c r="Z52" t="s">
-        <v>38</v>
+      <c r="Z52" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA52" t="s">
         <v>52</v>
@@ -5935,10 +5904,10 @@
         <v>3007570.6329999999</v>
       </c>
       <c r="B53" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C53" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D53" t="s">
         <v>35</v>
@@ -5950,7 +5919,7 @@
         <v>37</v>
       </c>
       <c r="G53" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H53">
         <v>90</v>
@@ -6006,8 +5975,8 @@
       <c r="Y53" t="s">
         <v>38</v>
       </c>
-      <c r="Z53" t="s">
-        <v>38</v>
+      <c r="Z53" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA53" t="s">
         <v>52</v>
@@ -6036,10 +6005,10 @@
         <v>3022053.1129999999</v>
       </c>
       <c r="B54" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D54" t="s">
         <v>35</v>
@@ -6051,7 +6020,7 @@
         <v>37</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H54">
         <v>100</v>
@@ -6107,8 +6076,8 @@
       <c r="Y54" t="s">
         <v>38</v>
       </c>
-      <c r="Z54" t="s">
-        <v>38</v>
+      <c r="Z54" s="1">
+        <v>1</v>
       </c>
       <c r="AA54" t="s">
         <v>52</v>
@@ -6137,10 +6106,10 @@
         <v>3036535.5920000002</v>
       </c>
       <c r="B55" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C55" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D55" t="s">
         <v>35</v>
@@ -6208,8 +6177,8 @@
       <c r="Y55" t="s">
         <v>38</v>
       </c>
-      <c r="Z55" t="s">
-        <v>38</v>
+      <c r="Z55" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA55" t="s">
         <v>52</v>
@@ -6238,10 +6207,10 @@
         <v>3051018.0720000002</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C56" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="D56" t="s">
         <v>35</v>
@@ -6309,8 +6278,8 @@
       <c r="Y56" t="s">
         <v>38</v>
       </c>
-      <c r="Z56" t="s">
-        <v>38</v>
+      <c r="Z56" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA56" t="s">
         <v>52</v>
@@ -6339,10 +6308,10 @@
         <v>3065500.5520000001</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D57" t="s">
         <v>35</v>
@@ -6354,7 +6323,7 @@
         <v>37</v>
       </c>
       <c r="G57" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H57">
         <v>40</v>
@@ -6410,8 +6379,8 @@
       <c r="Y57" t="s">
         <v>38</v>
       </c>
-      <c r="Z57" t="s">
-        <v>38</v>
+      <c r="Z57" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA57" t="s">
         <v>52</v>
@@ -6440,10 +6409,10 @@
         <v>3079983.0320000001</v>
       </c>
       <c r="B58" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
         <v>35</v>
@@ -6455,7 +6424,7 @@
         <v>37</v>
       </c>
       <c r="G58" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H58">
         <v>80</v>
@@ -6511,8 +6480,8 @@
       <c r="Y58" t="s">
         <v>38</v>
       </c>
-      <c r="Z58" t="s">
-        <v>38</v>
+      <c r="Z58" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA58" t="s">
         <v>52</v>
@@ -6541,10 +6510,10 @@
         <v>3094465.5120000001</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>
@@ -6556,7 +6525,7 @@
         <v>37</v>
       </c>
       <c r="G59" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H59">
         <v>100</v>
@@ -6612,8 +6581,8 @@
       <c r="Y59" t="s">
         <v>38</v>
       </c>
-      <c r="Z59" t="s">
-        <v>38</v>
+      <c r="Z59" s="1">
+        <v>1</v>
       </c>
       <c r="AA59" t="s">
         <v>52</v>
@@ -6642,10 +6611,10 @@
         <v>3108947.9920000001</v>
       </c>
       <c r="B60" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="D60" t="s">
         <v>35</v>
@@ -6713,8 +6682,8 @@
       <c r="Y60" t="s">
         <v>38</v>
       </c>
-      <c r="Z60" t="s">
-        <v>38</v>
+      <c r="Z60" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA60" t="s">
         <v>52</v>
@@ -6743,10 +6712,10 @@
         <v>3123430.4709999999</v>
       </c>
       <c r="B61" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="D61" t="s">
         <v>35</v>
@@ -6814,8 +6783,8 @@
       <c r="Y61" t="s">
         <v>38</v>
       </c>
-      <c r="Z61" t="s">
-        <v>38</v>
+      <c r="Z61" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA61" t="s">
         <v>52</v>
@@ -6844,10 +6813,10 @@
         <v>3137912.9509999999</v>
       </c>
       <c r="B62" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D62" t="s">
         <v>35</v>
@@ -6859,7 +6828,7 @@
         <v>37</v>
       </c>
       <c r="G62" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H62">
         <v>100</v>
@@ -6915,8 +6884,8 @@
       <c r="Y62" t="s">
         <v>38</v>
       </c>
-      <c r="Z62" t="s">
-        <v>38</v>
+      <c r="Z62" s="1">
+        <v>1</v>
       </c>
       <c r="AA62" t="s">
         <v>52</v>
@@ -6945,10 +6914,10 @@
         <v>3152395.4309999999</v>
       </c>
       <c r="B63" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D63" t="s">
         <v>35</v>
@@ -6960,7 +6929,7 @@
         <v>37</v>
       </c>
       <c r="G63" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H63">
         <v>61</v>
@@ -7016,8 +6985,8 @@
       <c r="Y63" t="s">
         <v>38</v>
       </c>
-      <c r="Z63" t="s">
-        <v>38</v>
+      <c r="Z63" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA63" t="s">
         <v>52</v>
@@ -7046,10 +7015,10 @@
         <v>3166877.9109999998</v>
       </c>
       <c r="B64" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="D64" t="s">
         <v>35</v>
@@ -7061,7 +7030,7 @@
         <v>37</v>
       </c>
       <c r="G64" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H64">
         <v>30</v>
@@ -7117,8 +7086,8 @@
       <c r="Y64" t="s">
         <v>38</v>
       </c>
-      <c r="Z64" t="s">
-        <v>38</v>
+      <c r="Z64" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA64" t="s">
         <v>52</v>
@@ -7147,10 +7116,10 @@
         <v>3181360.3909999998</v>
       </c>
       <c r="B65" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="C65" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D65" t="s">
         <v>35</v>
@@ -7218,8 +7187,8 @@
       <c r="Y65" t="s">
         <v>38</v>
       </c>
-      <c r="Z65" t="s">
-        <v>38</v>
+      <c r="Z65" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA65" t="s">
         <v>52</v>
@@ -7248,10 +7217,10 @@
         <v>3195842.8709999998</v>
       </c>
       <c r="B66" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D66" t="s">
         <v>35</v>
@@ -7319,8 +7288,8 @@
       <c r="Y66" t="s">
         <v>38</v>
       </c>
-      <c r="Z66" t="s">
-        <v>38</v>
+      <c r="Z66" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA66" t="s">
         <v>52</v>
@@ -7349,10 +7318,10 @@
         <v>3210325.3509999998</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="D67" t="s">
         <v>35</v>
@@ -7364,7 +7333,7 @@
         <v>37</v>
       </c>
       <c r="G67" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H67">
         <v>100</v>
@@ -7420,8 +7389,8 @@
       <c r="Y67" t="s">
         <v>38</v>
       </c>
-      <c r="Z67" t="s">
-        <v>38</v>
+      <c r="Z67" s="1">
+        <v>1</v>
       </c>
       <c r="AA67" t="s">
         <v>52</v>
@@ -7450,10 +7419,10 @@
         <v>3224807.83</v>
       </c>
       <c r="B68" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C68" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D68" t="s">
         <v>35</v>
@@ -7462,7 +7431,7 @@
         <v>37</v>
       </c>
       <c r="G68" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H68">
         <v>100</v>
@@ -7518,8 +7487,8 @@
       <c r="Y68" t="s">
         <v>38</v>
       </c>
-      <c r="Z68" t="s">
-        <v>38</v>
+      <c r="Z68" s="1">
+        <v>1</v>
       </c>
       <c r="AA68" t="s">
         <v>52</v>
@@ -7548,10 +7517,10 @@
         <v>3239290.31</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="D69" t="s">
         <v>35</v>
@@ -7563,7 +7532,7 @@
         <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H69" t="s">
         <v>39</v>
@@ -7619,8 +7588,8 @@
       <c r="Y69" t="s">
         <v>38</v>
       </c>
-      <c r="Z69" t="s">
-        <v>38</v>
+      <c r="Z69" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="AA69" t="s">
         <v>52</v>
@@ -7649,10 +7618,10 @@
         <v>3253772.79</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="E70" t="s">
         <v>36</v>
@@ -7717,8 +7686,8 @@
       <c r="Y70" t="s">
         <v>38</v>
       </c>
-      <c r="Z70" t="s">
-        <v>38</v>
+      <c r="Z70" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA70" t="s">
         <v>52</v>
@@ -7747,10 +7716,10 @@
         <v>3268255.27</v>
       </c>
       <c r="B71" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="C71" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="D71" t="s">
         <v>35</v>
@@ -7818,8 +7787,8 @@
       <c r="Y71" t="s">
         <v>38</v>
       </c>
-      <c r="Z71" t="s">
-        <v>38</v>
+      <c r="Z71" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA71" t="s">
         <v>52</v>
@@ -7848,10 +7817,10 @@
         <v>3282737.75</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D72" t="s">
         <v>35</v>
@@ -7863,7 +7832,7 @@
         <v>37</v>
       </c>
       <c r="G72" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H72">
         <v>100</v>
@@ -7919,8 +7888,8 @@
       <c r="Y72" t="s">
         <v>38</v>
       </c>
-      <c r="Z72" t="s">
-        <v>38</v>
+      <c r="Z72" s="1">
+        <v>1</v>
       </c>
       <c r="AA72" t="s">
         <v>52</v>
@@ -7949,10 +7918,10 @@
         <v>3297220.23</v>
       </c>
       <c r="B73" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
         <v>35</v>
@@ -7961,7 +7930,7 @@
         <v>36</v>
       </c>
       <c r="G73" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H73">
         <v>61</v>
@@ -8017,8 +7986,8 @@
       <c r="Y73" t="s">
         <v>38</v>
       </c>
-      <c r="Z73" t="s">
-        <v>38</v>
+      <c r="Z73" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA73" t="s">
         <v>52</v>
@@ -8047,7 +8016,7 @@
         <v>3311702.7089999998</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D74" t="s">
         <v>35</v>
@@ -8059,7 +8028,7 @@
         <v>37</v>
       </c>
       <c r="G74" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H74">
         <v>30</v>
@@ -8115,8 +8084,8 @@
       <c r="Y74" t="s">
         <v>38</v>
       </c>
-      <c r="Z74" t="s">
-        <v>38</v>
+      <c r="Z74" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA74" t="s">
         <v>52</v>
@@ -8145,10 +8114,10 @@
         <v>3326185.1889999998</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D75" t="s">
         <v>35</v>
@@ -8216,8 +8185,8 @@
       <c r="Y75" t="s">
         <v>38</v>
       </c>
-      <c r="Z75" t="s">
-        <v>38</v>
+      <c r="Z75" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA75" t="s">
         <v>52</v>
@@ -8246,10 +8215,10 @@
         <v>3340667.6690000002</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D76" t="s">
         <v>35</v>
@@ -8317,8 +8286,8 @@
       <c r="Y76" t="s">
         <v>38</v>
       </c>
-      <c r="Z76" t="s">
-        <v>38</v>
+      <c r="Z76" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA76" t="s">
         <v>52</v>
@@ -8347,10 +8316,10 @@
         <v>3355150.1490000002</v>
       </c>
       <c r="B77" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="C77" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
         <v>35</v>
@@ -8362,7 +8331,7 @@
         <v>37</v>
       </c>
       <c r="G77" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H77">
         <v>100</v>
@@ -8418,8 +8387,8 @@
       <c r="Y77" t="s">
         <v>38</v>
       </c>
-      <c r="Z77" t="s">
-        <v>38</v>
+      <c r="Z77" s="1">
+        <v>1</v>
       </c>
       <c r="AA77" t="s">
         <v>52</v>
@@ -8448,10 +8417,10 @@
         <v>3369632.6290000002</v>
       </c>
       <c r="B78" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="D78" t="s">
         <v>35</v>
@@ -8463,7 +8432,7 @@
         <v>37</v>
       </c>
       <c r="G78" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H78" t="s">
         <v>47</v>
@@ -8519,8 +8488,8 @@
       <c r="Y78" t="s">
         <v>38</v>
       </c>
-      <c r="Z78" t="s">
-        <v>38</v>
+      <c r="Z78" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA78" t="s">
         <v>52</v>
@@ -8549,7 +8518,7 @@
         <v>3384115.1090000002</v>
       </c>
       <c r="C79" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="D79" t="s">
         <v>35</v>
@@ -8561,7 +8530,7 @@
         <v>37</v>
       </c>
       <c r="G79" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H79">
         <v>90</v>
@@ -8617,8 +8586,8 @@
       <c r="Y79" t="s">
         <v>38</v>
       </c>
-      <c r="Z79" t="s">
-        <v>38</v>
+      <c r="Z79" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA79" t="s">
         <v>52</v>
@@ -8647,10 +8616,10 @@
         <v>3398597.5890000002</v>
       </c>
       <c r="B80" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D80" t="s">
         <v>35</v>
@@ -8718,8 +8687,8 @@
       <c r="Y80" t="s">
         <v>38</v>
       </c>
-      <c r="Z80" t="s">
-        <v>38</v>
+      <c r="Z80" s="1">
+        <v>1</v>
       </c>
       <c r="AA80" t="s">
         <v>52</v>
@@ -8748,10 +8717,10 @@
         <v>3413080.068</v>
       </c>
       <c r="B81" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C81" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D81" t="s">
         <v>35</v>
@@ -8819,8 +8788,8 @@
       <c r="Y81" t="s">
         <v>38</v>
       </c>
-      <c r="Z81" t="s">
-        <v>38</v>
+      <c r="Z81" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA81" t="s">
         <v>52</v>
@@ -8849,10 +8818,10 @@
         <v>3427562.548</v>
       </c>
       <c r="B82" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C82" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="D82" t="s">
         <v>35</v>
@@ -8861,7 +8830,7 @@
         <v>36</v>
       </c>
       <c r="G82" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H82">
         <v>30</v>
@@ -8917,8 +8886,8 @@
       <c r="Y82" t="s">
         <v>38</v>
       </c>
-      <c r="Z82" t="s">
-        <v>38</v>
+      <c r="Z82" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA82" t="s">
         <v>52</v>
@@ -8947,7 +8916,7 @@
         <v>3442045.0279999999</v>
       </c>
       <c r="C83" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="D83" t="s">
         <v>35</v>
@@ -8959,7 +8928,7 @@
         <v>37</v>
       </c>
       <c r="G83" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H83">
         <v>40</v>
@@ -9015,8 +8984,8 @@
       <c r="Y83" t="s">
         <v>38</v>
       </c>
-      <c r="Z83" t="s">
-        <v>38</v>
+      <c r="Z83" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA83" t="s">
         <v>52</v>
@@ -9045,10 +9014,10 @@
         <v>3456527.5079999999</v>
       </c>
       <c r="B84" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C84" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="D84" t="s">
         <v>35</v>
@@ -9060,7 +9029,7 @@
         <v>37</v>
       </c>
       <c r="G84" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H84">
         <v>80</v>
@@ -9116,8 +9085,8 @@
       <c r="Y84" t="s">
         <v>38</v>
       </c>
-      <c r="Z84" t="s">
-        <v>38</v>
+      <c r="Z84" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA84" t="s">
         <v>52</v>
@@ -9146,10 +9115,10 @@
         <v>3471009.9879999999</v>
       </c>
       <c r="B85" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C85" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D85" t="s">
         <v>35</v>
@@ -9217,8 +9186,8 @@
       <c r="Y85" t="s">
         <v>38</v>
       </c>
-      <c r="Z85" t="s">
-        <v>38</v>
+      <c r="Z85" s="1">
+        <v>1</v>
       </c>
       <c r="AA85" t="s">
         <v>52</v>
@@ -9247,10 +9216,10 @@
         <v>3485492.4679999999</v>
       </c>
       <c r="B86" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="C86" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D86" t="s">
         <v>35</v>
@@ -9318,8 +9287,8 @@
       <c r="Y86" t="s">
         <v>38</v>
       </c>
-      <c r="Z86" t="s">
-        <v>38</v>
+      <c r="Z86" s="1">
+        <v>1</v>
       </c>
       <c r="AA86" t="s">
         <v>52</v>
@@ -9348,10 +9317,10 @@
         <v>3499974.9470000002</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="C87" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="D87" t="s">
         <v>35</v>
@@ -9363,7 +9332,7 @@
         <v>37</v>
       </c>
       <c r="G87" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H87" t="s">
         <v>39</v>
@@ -9419,8 +9388,8 @@
       <c r="Y87" t="s">
         <v>38</v>
       </c>
-      <c r="Z87" t="s">
-        <v>38</v>
+      <c r="Z87" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="AA87" t="s">
         <v>52</v>
@@ -9449,10 +9418,10 @@
         <v>3514457.4270000001</v>
       </c>
       <c r="B88" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="C88" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="D88" t="s">
         <v>35</v>
@@ -9464,7 +9433,7 @@
         <v>37</v>
       </c>
       <c r="G88" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H88" t="s">
         <v>47</v>
@@ -9520,8 +9489,8 @@
       <c r="Y88" t="s">
         <v>38</v>
       </c>
-      <c r="Z88" t="s">
-        <v>38</v>
+      <c r="Z88" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA88" t="s">
         <v>52</v>
@@ -9550,10 +9519,10 @@
         <v>3528939.9070000001</v>
       </c>
       <c r="B89" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="C89" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="D89" t="s">
         <v>35</v>
@@ -9565,7 +9534,7 @@
         <v>37</v>
       </c>
       <c r="G89" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H89">
         <v>90</v>
@@ -9621,8 +9590,8 @@
       <c r="Y89" t="s">
         <v>38</v>
       </c>
-      <c r="Z89" t="s">
-        <v>38</v>
+      <c r="Z89" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA89" t="s">
         <v>52</v>
@@ -9651,10 +9620,10 @@
         <v>3543422.3870000001</v>
       </c>
       <c r="B90" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="D90" t="s">
         <v>35</v>
@@ -9722,8 +9691,8 @@
       <c r="Y90" t="s">
         <v>38</v>
       </c>
-      <c r="Z90" t="s">
-        <v>38</v>
+      <c r="Z90" s="1">
+        <v>1</v>
       </c>
       <c r="AA90" t="s">
         <v>52</v>
@@ -9752,10 +9721,10 @@
         <v>3557904.8670000001</v>
       </c>
       <c r="B91" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="C91" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="D91" t="s">
         <v>35</v>
@@ -9823,8 +9792,8 @@
       <c r="Y91" t="s">
         <v>38</v>
       </c>
-      <c r="Z91" t="s">
-        <v>38</v>
+      <c r="Z91" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA91" t="s">
         <v>52</v>
@@ -9853,10 +9822,10 @@
         <v>3572387.3470000001</v>
       </c>
       <c r="B92" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="C92" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D92" t="s">
         <v>35</v>
@@ -9868,7 +9837,7 @@
         <v>37</v>
       </c>
       <c r="G92" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H92">
         <v>30</v>
@@ -9924,8 +9893,8 @@
       <c r="Y92" t="s">
         <v>38</v>
       </c>
-      <c r="Z92" t="s">
-        <v>38</v>
+      <c r="Z92" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA92" t="s">
         <v>52</v>
@@ -9954,10 +9923,10 @@
         <v>3586869.8259999999</v>
       </c>
       <c r="B93" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="C93" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D93" t="s">
         <v>35</v>
@@ -9969,7 +9938,7 @@
         <v>37</v>
       </c>
       <c r="G93" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H93">
         <v>40</v>
@@ -10025,8 +9994,8 @@
       <c r="Y93" t="s">
         <v>38</v>
       </c>
-      <c r="Z93" t="s">
-        <v>38</v>
+      <c r="Z93" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA93" t="s">
         <v>52</v>
@@ -10055,10 +10024,10 @@
         <v>3601352.3059999999</v>
       </c>
       <c r="B94" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C94" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D94" t="s">
         <v>35</v>
@@ -10070,7 +10039,7 @@
         <v>37</v>
       </c>
       <c r="G94" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H94">
         <v>80</v>
@@ -10126,8 +10095,8 @@
       <c r="Y94" t="s">
         <v>38</v>
       </c>
-      <c r="Z94" t="s">
-        <v>38</v>
+      <c r="Z94" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="AA94" t="s">
         <v>52</v>
@@ -10156,7 +10125,7 @@
         <v>3615834.7859999998</v>
       </c>
       <c r="C95" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="D95" t="s">
         <v>35</v>
@@ -10221,8 +10190,8 @@
       <c r="Y95" t="s">
         <v>38</v>
       </c>
-      <c r="Z95" t="s">
-        <v>38</v>
+      <c r="Z95" s="1">
+        <v>1</v>
       </c>
       <c r="AA95" t="s">
         <v>52</v>
@@ -10251,10 +10220,10 @@
         <v>3630317.2659999998</v>
       </c>
       <c r="B96" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="C96" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D96" t="s">
         <v>35</v>
@@ -10322,8 +10291,8 @@
       <c r="Y96" t="s">
         <v>38</v>
       </c>
-      <c r="Z96" t="s">
-        <v>38</v>
+      <c r="Z96" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="AA96" t="s">
         <v>52</v>
@@ -10352,10 +10321,10 @@
         <v>3644799.7459999998</v>
       </c>
       <c r="B97" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="C97" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="E97" t="s">
         <v>36</v>
@@ -10364,7 +10333,7 @@
         <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H97">
         <v>90</v>
@@ -10420,8 +10389,8 @@
       <c r="Y97" t="s">
         <v>38</v>
       </c>
-      <c r="Z97" t="s">
-        <v>38</v>
+      <c r="Z97" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="AA97" t="s">
         <v>52</v>
@@ -10450,10 +10419,10 @@
         <v>3659282.2259999998</v>
       </c>
       <c r="B98" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="C98" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="D98" t="s">
         <v>35</v>
@@ -10465,7 +10434,7 @@
         <v>37</v>
       </c>
       <c r="G98" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H98">
         <v>100</v>
@@ -10521,8 +10490,8 @@
       <c r="Y98" t="s">
         <v>38</v>
       </c>
-      <c r="Z98" t="s">
-        <v>38</v>
+      <c r="Z98" s="1">
+        <v>1</v>
       </c>
       <c r="AA98" t="s">
         <v>52</v>
@@ -10551,10 +10520,10 @@
         <v>3673764.7059999998</v>
       </c>
       <c r="B99" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="C99" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="D99" t="s">
         <v>35</v>
@@ -10566,7 +10535,7 @@
         <v>37</v>
       </c>
       <c r="G99" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H99">
         <v>61</v>
@@ -10622,8 +10591,8 @@
       <c r="Y99" t="s">
         <v>38</v>
       </c>
-      <c r="Z99" t="s">
-        <v>38</v>
+      <c r="Z99" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="AA99" t="s">
         <v>52</v>
@@ -10652,10 +10621,10 @@
         <v>3688247.1850000001</v>
       </c>
       <c r="B100" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="C100" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="D100" t="s">
         <v>35</v>
@@ -10723,8 +10692,8 @@
       <c r="Y100" t="s">
         <v>38</v>
       </c>
-      <c r="Z100" t="s">
-        <v>38</v>
+      <c r="Z100" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="AA100" t="s">
         <v>52</v>
@@ -10753,10 +10722,10 @@
         <v>3702729.665</v>
       </c>
       <c r="B101" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="C101" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="D101" t="s">
         <v>35</v>
@@ -10824,8 +10793,8 @@
       <c r="Y101" t="s">
         <v>38</v>
       </c>
-      <c r="Z101" t="s">
-        <v>38</v>
+      <c r="Z101" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="AA101" t="s">
         <v>52</v>

</xml_diff>